<commit_message>
more mapping and mapping documentation updating
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF516B7-DD51-4E50-9E10-B172411BBC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3B57D-BA5E-4EF5-8C1B-4D3B79CAD14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,160 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jack Mangano</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{7C1260E7-6BF4-4C49-B6DF-E10333CE8A6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{8A710AE6-B83F-4E7B-9641-D9BE1F35E473}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{4CBE1649-23DD-48DE-9FCB-4776AA279031}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Region : region1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{C182412E-0F6B-4597-B1EC-5EE18E511E43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{01AD695C-A6D5-455D-B860-12480091417F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Region : region1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{BF44C95C-147F-4675-9003-A989C359C1F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56,13 +210,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,6 +269,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8F1DA6-05E6-4E4D-9C8A-17115F54DD67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8F1DA6-05E6-4E4D-9C8A-17115F54DD67}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,20 +588,20 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>2</v>
       </c>
     </row>
@@ -441,7 +612,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>11</v>
       </c>
     </row>
@@ -449,7 +620,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="D4">
         <v>12</v>
       </c>
     </row>
@@ -457,6 +631,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -495,6 +672,9 @@
       <c r="B12">
         <v>3</v>
       </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -506,5 +686,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added conditional color formatting to map excel sheet
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3A348E-DB6B-4DB6-AF46-FC322F431C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4FC578-7EFE-440E-A3B1-5A543516A548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
@@ -364,8 +364,373 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF666699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF993366"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF993366"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF666699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF666699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF993366"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF993366"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF006600"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF666699"/>
+      <color rgb="FF993366"/>
+      <color rgb="FFFF0066"/>
+      <color rgb="FFFF3300"/>
+      <color rgb="FF3366FF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFCC0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -681,7 +1046,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +1159,48 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E13">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:E13">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more room connections. walk cycle animation fix.
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06B0EA6-31E6-4F4B-A0B6-E04DCC3863A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39844FC1-A576-4978-A784-0106E71814BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2nd floor" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -215,6 +215,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{D38A2BC3-F417-47C6-B901-A7EC2E659F7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B12" authorId="0" shapeId="0" xr:uid="{30A31D7F-3E40-42C6-A53F-6A24F1ADC598}">
       <text>
         <r>
@@ -336,7 +360,7 @@
           </rPr>
           <t xml:space="preserve">
 Hotspot : hExit1
-</t>
+5, 314, 115, eDirectionLeft</t>
         </r>
       </text>
     </comment>
@@ -362,6 +386,56 @@
           <t xml:space="preserve">
 Region : region1
 2, 5, 115, eDirectionRight</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{BCEA3F34-39AF-4290-8032-FF806D9EE781}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1
+2, 5, 115, eDirectionRight</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{A637598B-FF0F-477B-A7A4-657F4EE29819}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Region : region1
+5, 5, 115, eDirectionLeft</t>
         </r>
       </text>
     </comment>
@@ -481,7 +555,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -577,594 +658,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF996633"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF666699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF993366"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1193,10 +686,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1499,7 +988,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:E15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1064,9 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1">
@@ -1679,49 +1170,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E570">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
last check-in of changes for 3/30/2022
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC730FB7-E27E-4AC8-A2D2-8D48BFB69341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F3B67-B064-456D-80A3-D3B4EF852E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
   <sheets>
     <sheet name="2nd floor" sheetId="1" r:id="rId1"/>
@@ -315,6 +315,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{17B616B5-564B-4390-A991-74A5B26817BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Region : region1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B12" authorId="0" shapeId="0" xr:uid="{30A31D7F-3E40-42C6-A53F-6A24F1ADC598}">
       <text>
         <r>
@@ -515,6 +539,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{1C1D2EFD-8F0B-490E-B700-44DADA51BF44}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E16" authorId="0" shapeId="0" xr:uid="{C000348B-41C4-40F5-BF42-D2AF55D5516A}">
       <text>
         <r>
@@ -537,6 +585,30 @@
           <t xml:space="preserve">
 Region : region1
 5, 5, 115, eDirectionRight</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{1A7B4B1C-8F82-40E7-B783-6C984EA07CE2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Region : region1</t>
         </r>
       </text>
     </comment>
@@ -644,7 +716,126 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8E7300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF996633"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF993366"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF666699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -866,6 +1057,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FF8E7300"/>
       <color rgb="FFFFCC00"/>
       <color rgb="FF996633"/>
@@ -875,7 +1067,6 @@
       <color rgb="FF993366"/>
       <color rgb="FFFF0066"/>
       <color rgb="FFFF3300"/>
-      <color rgb="FF3366FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1189,7 +1380,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1485,9 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1379,7 +1572,9 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>7</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2">
@@ -1387,10 +1582,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>7</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,53 +1720,56 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E570">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Room Number Debug Objects
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E07704-9578-42AA-BFE5-26C05C03C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03FDAB-D62A-49D3-92A0-8BEDF070799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
@@ -1162,7 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8F1DA6-05E6-4E4D-9C8A-17115F54DD67}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
we animating more rooms
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03FDAB-D62A-49D3-92A0-8BEDF070799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71E278-88D5-4C29-B87D-BF4D3053D158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
made a ton of changes. fixed font. learned things.
</commit_message>
<xml_diff>
--- a/data/rooms/map.xlsx
+++ b/data/rooms/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71E278-88D5-4C29-B87D-BF4D3053D158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD585F3C-D7A2-466C-9AEE-8E4E892EB3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20A55568-D4B8-4FF3-B18F-5DDC70E2225A}"/>
   </bookViews>
   <sheets>
     <sheet name="2nd floor" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Hotspot : hExit1</t>
+Hotspot : hExit1
+7, 314, 115, eDirectionLeft</t>
         </r>
       </text>
     </comment>
@@ -588,6 +589,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{1A3329C7-F091-4FD8-90DB-581218510878}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jack Mangano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hotspot : hExit1
+5, 5, 115, eDirectionRight</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D17" authorId="0" shapeId="0" xr:uid="{1A7B4B1C-8F82-40E7-B783-6C984EA07CE2}">
       <text>
         <r>
@@ -608,7 +634,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Region : region1</t>
+Region : region1
+7, 314, 115, eDirectionLeft</t>
         </r>
       </text>
     </comment>
@@ -861,6 +888,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,7 +1194,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1399,9 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>7</v>

</xml_diff>